<commit_message>
fix date in db
</commit_message>
<xml_diff>
--- a/dl/obligation/Parametry_vypuska_OFZ-n_53007_2.xlsx
+++ b/dl/obligation/Parametry_vypuska_OFZ-n_53007_2.xlsx
@@ -417,11 +417,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -449,11 +449,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -488,7 +488,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,7 +501,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.7"/>
@@ -509,7 +509,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -993,7 +993,7 @@
         <v>198</v>
       </c>
       <c r="D35" s="14" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E35" s="15" t="n">
         <v>21.7</v>
@@ -1016,7 +1016,7 @@
         <v>182</v>
       </c>
       <c r="D36" s="14" t="n">
-        <v>0.044</v>
+        <v>4.4</v>
       </c>
       <c r="E36" s="15" t="n">
         <v>21.94</v>
@@ -1039,7 +1039,7 @@
         <v>182</v>
       </c>
       <c r="D37" s="14" t="n">
-        <v>0.049</v>
+        <v>4.9</v>
       </c>
       <c r="E37" s="15" t="n">
         <v>24.43</v>
@@ -1065,7 +1065,7 @@
         <v>182</v>
       </c>
       <c r="D38" s="14" t="n">
-        <v>0.0545</v>
+        <v>5.45</v>
       </c>
       <c r="E38" s="15" t="n">
         <v>27.18</v>
@@ -1089,7 +1089,7 @@
         <v>182</v>
       </c>
       <c r="D39" s="14" t="n">
-        <v>0.0605</v>
+        <v>6.05</v>
       </c>
       <c r="E39" s="15" t="n">
         <v>30.17</v>
@@ -1111,7 +1111,7 @@
         <v>182</v>
       </c>
       <c r="D40" s="14" t="n">
-        <v>0.0675</v>
+        <v>6.75</v>
       </c>
       <c r="E40" s="15" t="n">
         <v>33.66</v>

</xml_diff>